<commit_message>
After updating test case name
</commit_message>
<xml_diff>
--- a/tricentis-web-app.XLSX
+++ b/tricentis-web-app.XLSX
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Gender</t>
   </si>
@@ -42,6 +42,66 @@
   </si>
   <si>
     <t>divya.k@0612</t>
+  </si>
+  <si>
+    <t>Checkout Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Address : </t>
+  </si>
+  <si>
+    <t>9361844977</t>
+  </si>
+  <si>
+    <t>Bahwan Cybertek</t>
+  </si>
+  <si>
+    <t>1st main road, Subbarayan nagar</t>
+  </si>
+  <si>
+    <t>Thoraipakkam</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>600097</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment method : </t>
+  </si>
+  <si>
+    <t>CashOnDelivery</t>
+  </si>
+  <si>
+    <t>Product Detailes</t>
+  </si>
+  <si>
+    <t>Music 2</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>Not required</t>
+  </si>
+  <si>
+    <t>7.00</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>27.00</t>
   </si>
 </sst>
 </file>
@@ -86,7 +146,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,6 +168,9 @@
       <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
@@ -124,6 +187,119 @@
       </c>
       <c r="E2" t="s" s="0">
         <v>9</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="F3" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="F4" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="F6" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="F7" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="F8" t="s" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="F9" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="F10" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="F11" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="F12" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="F13" t="s" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="F14" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="F15" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="F16" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="F17" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="F18" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="F19" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="F20" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="F21" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="F22" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="F23" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="F24" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>